<commit_message>
Restart to new implementation
</commit_message>
<xml_diff>
--- a/data/dummy_1.xlsx
+++ b/data/dummy_1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johnloyd/Desktop/OAA-DMS/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD86392D-8031-1C47-A17A-1546C331642B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FD15F8F-247A-D049-982E-308A8062190E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30460" yWindow="4060" windowWidth="30620" windowHeight="17440" xr2:uid="{A39F77A8-956E-254C-937C-9E03048B92EC}"/>
+    <workbookView xWindow="30460" yWindow="4060" windowWidth="30620" windowHeight="17440" activeTab="3" xr2:uid="{A39F77A8-956E-254C-937C-9E03048B92EC}"/>
   </bookViews>
   <sheets>
     <sheet name="Donor" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="104">
   <si>
     <t>id</t>
   </si>
@@ -337,13 +337,19 @@
     <t>purposeOfDonation</t>
   </si>
   <si>
-    <t>Equal to scholarship name?</t>
-  </si>
-  <si>
     <t>salutation</t>
   </si>
   <si>
     <t>Mr.</t>
+  </si>
+  <si>
+    <t>nothing</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>test</t>
   </si>
 </sst>
 </file>
@@ -388,10 +394,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -709,7 +716,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0274B901-3B17-4440-A6B6-1F424B94EA3E}">
   <dimension ref="A1:S4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -727,7 +734,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -786,7 +793,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>64</v>
@@ -835,7 +842,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>65</v>
@@ -884,7 +891,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>66</v>
@@ -1124,11 +1131,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4D55864-87A4-E94A-B2F1-27122E97EFB7}">
   <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="5" max="5" width="8.1640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -1178,8 +1188,29 @@
       <c r="A2">
         <v>1</v>
       </c>
+      <c r="C2">
+        <v>123456</v>
+      </c>
       <c r="D2" t="s">
-        <v>99</v>
+        <v>67</v>
+      </c>
+      <c r="F2">
+        <v>654321</v>
+      </c>
+      <c r="G2" s="3">
+        <v>44218</v>
+      </c>
+      <c r="H2">
+        <v>20000</v>
+      </c>
+      <c r="I2" t="s">
+        <v>101</v>
+      </c>
+      <c r="M2" t="s">
+        <v>102</v>
+      </c>
+      <c r="N2" t="s">
+        <v>103</v>
       </c>
     </row>
   </sheetData>

</xml_diff>